<commit_message>
Updated to September/October version
</commit_message>
<xml_diff>
--- a/agg_state/agg_state_2005_2006.xlsx
+++ b/agg_state/agg_state_2005_2006.xlsx
@@ -412,13 +412,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>-0.003</v>
+        <v>0.004</v>
       </c>
       <c r="B2">
-        <v>0.89</v>
+        <v>0.969</v>
       </c>
       <c r="C2">
-        <v>0.921</v>
+        <v>0.925</v>
       </c>
     </row>
   </sheetData>
@@ -447,13 +447,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>0.001</v>
+        <v>-0.009</v>
       </c>
       <c r="B2">
-        <v>0.931</v>
+        <v>0.827</v>
       </c>
       <c r="C2">
-        <v>0.92</v>
+        <v>0.919</v>
       </c>
     </row>
   </sheetData>
@@ -485,16 +485,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>0.003</v>
+        <v>-0.026</v>
       </c>
       <c r="B2">
-        <v>0.963</v>
+        <v>0.657</v>
       </c>
       <c r="C2">
-        <v>-294.5</v>
+        <v>2531.68</v>
       </c>
       <c r="D2">
-        <v>-0.003</v>
+        <v>0.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>